<commit_message>
modifiche test Ind_14, Ind_19, Ind_20
</commit_message>
<xml_diff>
--- a/earlywarning-pom/Document/test/RETAIL/test_Ind_High_Priority_RETAIL.xlsx
+++ b/earlywarning-pom/Document/test/RETAIL/test_Ind_High_Priority_RETAIL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="casistiche_indeterminate" sheetId="2" r:id="rId1"/>
     <sheet name="High_Priority" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="190">
   <si>
     <t>SNDG</t>
   </si>
@@ -596,8 +596,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -626,8 +626,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -649,6 +655,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -702,7 +714,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -726,9 +738,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -785,9 +794,6 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -803,9 +809,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1123,19 +1138,19 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="34" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="34"/>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="40"/>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>37</v>
       </c>
@@ -1143,13 +1158,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>40</v>
       </c>
@@ -1157,55 +1172,55 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="6"/>
       <c r="C9" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" s="6"/>
       <c r="C10" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" s="6"/>
       <c r="C11" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" s="6"/>
       <c r="C13" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="34" t="s">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="34"/>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C15" s="40"/>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>50</v>
       </c>
@@ -1213,19 +1228,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="6"/>
       <c r="C17" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="6"/>
       <c r="C18" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="6"/>
       <c r="C19" s="6" t="s">
         <v>51</v>
@@ -1244,54 +1259,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G123" sqref="G123"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="25.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="25.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="25.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="42.42578125" customWidth="1"/>
-    <col min="14" max="14" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="42.44140625" customWidth="1"/>
+    <col min="14" max="14" width="50.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="12" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>35</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="27" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1312,7 +1327,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -1336,7 +1351,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1357,43 +1372,43 @@
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="12" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="28" t="s">
+      <c r="H9" s="27" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
@@ -1414,7 +1429,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
@@ -1438,7 +1453,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>10</v>
       </c>
@@ -1459,43 +1474,43 @@
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="12" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="11" t="s">
         <v>53</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="28" t="s">
+      <c r="H16" s="27" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>8</v>
       </c>
@@ -1516,7 +1531,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
@@ -1540,7 +1555,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
       <c r="B19" s="5" t="s">
         <v>10</v>
@@ -1562,43 +1577,43 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="12" t="s">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B23" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="11" t="s">
         <v>19</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="11" t="s">
         <v>54</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="28" t="s">
+      <c r="H23" s="27" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
@@ -1619,7 +1634,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>13</v>
       </c>
@@ -1643,7 +1658,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
         <v>16</v>
       </c>
@@ -1664,51 +1679,51 @@
         <v>179</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="12" t="s">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B30" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="F30" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G30" s="12" t="s">
+      <c r="G30" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H30" s="12" t="s">
+      <c r="H30" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="I30" s="12" t="s">
+      <c r="I30" s="11" t="s">
         <v>29</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K30" s="12" t="s">
+      <c r="K30" s="11" t="s">
         <v>55</v>
       </c>
       <c r="L30" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M30" s="28" t="s">
+      <c r="M30" s="27" t="s">
         <v>183</v>
       </c>
-      <c r="N30" s="41" t="s">
+      <c r="N30" s="39" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
         <v>21</v>
       </c>
@@ -1745,37 +1760,37 @@
         <v>179</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="22">
+      <c r="C32" s="21">
         <v>100</v>
       </c>
-      <c r="D32" s="20">
-        <v>0</v>
-      </c>
-      <c r="E32" s="22">
+      <c r="D32" s="19">
+        <v>0</v>
+      </c>
+      <c r="E32" s="21">
         <v>1000</v>
       </c>
-      <c r="F32" s="22">
+      <c r="F32" s="21">
         <v>700</v>
       </c>
-      <c r="G32" s="22">
+      <c r="G32" s="21">
         <v>600</v>
       </c>
-      <c r="H32" s="22">
+      <c r="H32" s="21">
         <f t="shared" ref="H32:H38" si="0">D32-E32</f>
         <v>-1000</v>
       </c>
-      <c r="I32" s="22">
+      <c r="I32" s="21">
         <f t="shared" ref="I32:I37" si="1">MAX(F32,G32)</f>
         <v>700</v>
       </c>
-      <c r="J32" s="22">
+      <c r="J32" s="21">
         <v>100</v>
       </c>
       <c r="K32" s="4" t="s">
@@ -1788,7 +1803,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
         <v>23</v>
       </c>
@@ -1821,21 +1836,21 @@
       <c r="K33" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="L33" s="29" t="s">
+      <c r="L33" s="28" t="s">
         <v>56</v>
       </c>
       <c r="M33" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B34" s="5" t="s">
         <v>58</v>
       </c>
       <c r="C34" s="4">
         <v>0</v>
       </c>
-      <c r="D34" s="20">
+      <c r="D34" s="19">
         <v>1000</v>
       </c>
       <c r="E34" s="8">
@@ -1861,21 +1876,21 @@
       <c r="K34" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="L34" s="29" t="s">
+      <c r="L34" s="28" t="s">
         <v>56</v>
       </c>
       <c r="M34" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C35" s="4">
         <v>0</v>
       </c>
-      <c r="D35" s="20">
+      <c r="D35" s="19">
         <v>1000</v>
       </c>
       <c r="E35" s="8">
@@ -1901,21 +1916,21 @@
       <c r="K35" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="L35" s="29" t="s">
+      <c r="L35" s="28" t="s">
         <v>56</v>
       </c>
       <c r="M35" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="20">
+      <c r="D36" s="19">
         <v>1000</v>
       </c>
       <c r="E36" s="8">
@@ -1935,43 +1950,43 @@
         <f t="shared" si="1"/>
         <v>-10</v>
       </c>
-      <c r="J36" s="14">
+      <c r="J36" s="13">
         <v>-1000000</v>
       </c>
       <c r="K36" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L36" s="29" t="s">
+      <c r="L36" s="28" t="s">
         <v>57</v>
       </c>
       <c r="M36" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="35" t="s">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B37" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="36">
+      <c r="C37" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="34">
         <v>600</v>
       </c>
-      <c r="E37" s="37">
+      <c r="E37" s="35">
         <v>600</v>
       </c>
-      <c r="F37" s="38">
+      <c r="F37" s="36">
         <v>-10</v>
       </c>
-      <c r="G37" s="38">
+      <c r="G37" s="36">
         <v>-70</v>
       </c>
-      <c r="H37" s="38">
+      <c r="H37" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I37" s="38">
+      <c r="I37" s="36">
         <f t="shared" si="1"/>
         <v>-10</v>
       </c>
@@ -1983,14 +1998,14 @@
         <v>189</v>
       </c>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B38" s="5" t="s">
         <v>62</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="20">
+      <c r="D38" s="19">
         <v>-1000</v>
       </c>
       <c r="E38" s="8">
@@ -2010,27 +2025,27 @@
         <f>MAX(F38,G38)</f>
         <v>-10</v>
       </c>
-      <c r="J38" s="14">
+      <c r="J38" s="13">
         <v>-1000000</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L38" s="29" t="s">
+      <c r="L38" s="28" t="s">
         <v>57</v>
       </c>
       <c r="M38" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B39" s="5" t="s">
         <v>63</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D39" s="20">
+      <c r="D39" s="19">
         <v>1000</v>
       </c>
       <c r="E39" s="8">
@@ -2049,20 +2064,20 @@
         <f>MAX(F39,G39)</f>
         <v>0</v>
       </c>
-      <c r="J39" s="14">
+      <c r="J39" s="13">
         <v>-1000000</v>
       </c>
       <c r="K39" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L39" s="29" t="s">
+      <c r="L39" s="28" t="s">
         <v>57</v>
       </c>
       <c r="M39" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B40" s="5" t="s">
         <v>64</v>
       </c>
@@ -2087,20 +2102,20 @@
       <c r="I40" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="J40" s="14">
+      <c r="J40" s="13">
         <v>-1000000</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L40" s="29" t="s">
+      <c r="L40" s="28" t="s">
         <v>57</v>
       </c>
       <c r="M40" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B41" s="5" t="s">
         <v>66</v>
       </c>
@@ -2125,20 +2140,20 @@
       <c r="I41" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="J41" s="14">
+      <c r="J41" s="13">
         <v>-1000000</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L41" s="29" t="s">
+      <c r="L41" s="28" t="s">
         <v>57</v>
       </c>
       <c r="M41" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B42" s="5" t="s">
         <v>92</v>
       </c>
@@ -2163,24 +2178,24 @@
       <c r="I42" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="J42" s="14">
+      <c r="J42" s="13">
         <v>-1000000</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L42" s="29" t="s">
+      <c r="L42" s="28" t="s">
         <v>57</v>
       </c>
       <c r="M42" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B43" s="13" t="s">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B43" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C43" s="20" t="s">
+      <c r="C43" s="19" t="s">
         <v>5</v>
       </c>
       <c r="D43" s="4" t="s">
@@ -2208,72 +2223,72 @@
       <c r="K43" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L43" s="29" t="s">
+      <c r="L43" s="28" t="s">
         <v>57</v>
       </c>
       <c r="M43" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B44" s="39" t="s">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B44" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="C44" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="40" t="s">
+      <c r="C44" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="E44" s="38" t="s">
+      <c r="E44" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="F44" s="38">
+      <c r="F44" s="36">
         <v>-10</v>
       </c>
-      <c r="G44" s="38">
+      <c r="G44" s="36">
         <v>-70</v>
       </c>
-      <c r="H44" s="38" t="s">
+      <c r="H44" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="I44" s="38">
+      <c r="I44" s="36">
         <f>MAX(F44,G44)</f>
         <v>-10</v>
       </c>
-      <c r="J44" s="14"/>
+      <c r="J44" s="13"/>
       <c r="K44" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L44" s="29"/>
+      <c r="L44" s="28"/>
       <c r="M44" s="8"/>
       <c r="N44" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B45" s="39" t="s">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B45" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="C45" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="40" t="s">
+      <c r="C45" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="E45" s="38" t="s">
+      <c r="E45" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="F45" s="38">
-        <v>0</v>
-      </c>
-      <c r="G45" s="38">
+      <c r="F45" s="36">
+        <v>0</v>
+      </c>
+      <c r="G45" s="36">
         <v>-30</v>
       </c>
-      <c r="H45" s="38" t="s">
+      <c r="H45" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="I45" s="38">
+      <c r="I45" s="36">
         <f>MAX(F45,G45)</f>
         <v>0</v>
       </c>
@@ -2281,53 +2296,53 @@
       <c r="K45" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L45" s="29"/>
-      <c r="M45" s="22"/>
+      <c r="L45" s="28"/>
+      <c r="M45" s="21"/>
       <c r="N45" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="46" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="25"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="27"/>
-      <c r="H46" s="27"/>
-      <c r="I46" s="27"/>
-      <c r="J46" s="27"/>
-      <c r="K46" s="26"/>
-      <c r="L46" s="26"/>
-      <c r="M46" s="27"/>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="24"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
+      <c r="K46" s="25"/>
+      <c r="L46" s="25"/>
+      <c r="M46" s="26"/>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B48" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C48" s="12" t="s">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B48" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D48" s="12" t="s">
+      <c r="D48" s="11" t="s">
         <v>68</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F48" s="12" t="s">
+      <c r="F48" s="11" t="s">
         <v>69</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H48" s="28" t="s">
+      <c r="H48" s="27" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B49" s="5" t="s">
         <v>96</v>
       </c>
@@ -2348,7 +2363,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>67</v>
       </c>
@@ -2372,7 +2387,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B51" s="5" t="s">
         <v>98</v>
       </c>
@@ -2393,33 +2408,33 @@
         <v>179</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B53" s="1"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B54" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C54" s="12" t="s">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B54" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D54" s="12" t="s">
+      <c r="D54" s="11" t="s">
         <v>72</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F54" s="12" t="s">
+      <c r="F54" s="11" t="s">
         <v>73</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="H54" s="28" t="s">
+      <c r="H54" s="27" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B55" s="5" t="s">
         <v>99</v>
       </c>
@@ -2440,7 +2455,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>71</v>
       </c>
@@ -2464,7 +2479,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B57" s="5" t="s">
         <v>101</v>
       </c>
@@ -2477,7 +2492,7 @@
       <c r="E57" s="4">
         <v>0</v>
       </c>
-      <c r="F57" s="10" t="s">
+      <c r="F57" s="42" t="s">
         <v>75</v>
       </c>
       <c r="G57" s="8" t="s">
@@ -2487,30 +2502,30 @@
         <v>179</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B60" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C60" s="12" t="s">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B60" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D60" s="12" t="s">
+      <c r="D60" s="11" t="s">
         <v>76</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F60" s="12" t="s">
+      <c r="F60" s="11" t="s">
         <v>78</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="H60" s="28" t="s">
+      <c r="H60" s="27" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B61" s="5" t="s">
         <v>102</v>
       </c>
@@ -2531,7 +2546,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>77</v>
       </c>
@@ -2555,11 +2570,11 @@
         <v>179</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B63" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="C63" s="20">
+      <c r="C63" s="19">
         <v>0</v>
       </c>
       <c r="D63" s="4" t="s">
@@ -2575,34 +2590,34 @@
       <c r="H63" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="I63" s="19"/>
-      <c r="J63" s="19"/>
-      <c r="K63" s="19"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B66" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C66" s="12" t="s">
+      <c r="I63" s="18"/>
+      <c r="J63" s="18"/>
+      <c r="K63" s="18"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B66" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D66" s="12" t="s">
+      <c r="D66" s="11" t="s">
         <v>83</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F66" s="12" t="s">
+      <c r="F66" s="11" t="s">
         <v>81</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="H66" s="28" t="s">
+      <c r="H66" s="27" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B67" s="5" t="s">
         <v>104</v>
       </c>
@@ -2623,7 +2638,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>80</v>
       </c>
@@ -2647,7 +2662,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B69" s="5" t="s">
         <v>106</v>
       </c>
@@ -2667,35 +2682,35 @@
       <c r="H69" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="I69" s="19"/>
-      <c r="J69" s="19"/>
-      <c r="K69" s="19"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B72" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C72" s="12" t="s">
+      <c r="I69" s="18"/>
+      <c r="J69" s="18"/>
+      <c r="K69" s="18"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B72" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D72" s="12" t="s">
+      <c r="D72" s="11" t="s">
         <v>87</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F72" s="12" t="s">
+      <c r="F72" s="11" t="s">
         <v>85</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="H72" s="28" t="s">
+      <c r="H72" s="27" t="s">
         <v>183</v>
       </c>
-      <c r="I72" s="15"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I72" s="14"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B73" s="5" t="s">
         <v>107</v>
       </c>
@@ -2715,9 +2730,9 @@
       <c r="H73" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="I73" s="30"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I73" s="29"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>84</v>
       </c>
@@ -2741,7 +2756,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B75" s="5" t="s">
         <v>112</v>
       </c>
@@ -2761,37 +2776,37 @@
       <c r="H75" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="I75" s="19"/>
-      <c r="K75" s="19"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I76" s="23"/>
-      <c r="J76" s="27"/>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B78" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C78" s="12" t="s">
+      <c r="I75" s="18"/>
+      <c r="K75" s="18"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I76" s="22"/>
+      <c r="J76" s="26"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B78" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C78" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D78" s="12" t="s">
+      <c r="D78" s="11" t="s">
         <v>91</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F78" s="12" t="s">
+      <c r="F78" s="11" t="s">
         <v>89</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H78" s="28" t="s">
+      <c r="H78" s="27" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B79" s="5" t="s">
         <v>113</v>
       </c>
@@ -2811,10 +2826,10 @@
       <c r="H79" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="I79" s="16"/>
-      <c r="J79" s="16"/>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I79" s="15"/>
+      <c r="J79" s="15"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>88</v>
       </c>
@@ -2838,7 +2853,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B81" s="5" t="s">
         <v>117</v>
       </c>
@@ -2858,34 +2873,34 @@
       <c r="H81" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="I81" s="19"/>
-      <c r="J81" s="19"/>
-      <c r="K81" s="19"/>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B84" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C84" s="12" t="s">
+      <c r="I81" s="18"/>
+      <c r="J81" s="18"/>
+      <c r="K81" s="18"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B84" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C84" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D84" s="12" t="s">
+      <c r="D84" s="11" t="s">
         <v>115</v>
       </c>
       <c r="E84" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="F84" s="12" t="s">
+      <c r="F84" s="11" t="s">
         <v>110</v>
       </c>
       <c r="G84" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="H84" s="28" t="s">
+      <c r="H84" s="27" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B85" s="5" t="s">
         <v>118</v>
       </c>
@@ -2906,7 +2921,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>109</v>
       </c>
@@ -2930,7 +2945,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B87" s="5" t="s">
         <v>126</v>
       </c>
@@ -2943,7 +2958,9 @@
       <c r="E87" s="4">
         <v>0</v>
       </c>
-      <c r="F87" s="4"/>
+      <c r="F87" s="41" t="s">
+        <v>75</v>
+      </c>
       <c r="G87" s="4" t="s">
         <v>5</v>
       </c>
@@ -2951,30 +2968,30 @@
         <v>179</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B90" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C90" s="12" t="s">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B90" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C90" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D90" s="12" t="s">
+      <c r="D90" s="11" t="s">
         <v>116</v>
       </c>
       <c r="E90" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="F90" s="12" t="s">
+      <c r="F90" s="11" t="s">
         <v>121</v>
       </c>
       <c r="G90" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="H90" s="28" t="s">
+      <c r="H90" s="27" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B91" s="5" t="s">
         <v>127</v>
       </c>
@@ -2995,7 +3012,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>120</v>
       </c>
@@ -3019,7 +3036,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B93" s="5" t="s">
         <v>133</v>
       </c>
@@ -3032,7 +3049,9 @@
       <c r="E93" s="4">
         <v>0</v>
       </c>
-      <c r="F93" s="4"/>
+      <c r="F93" s="42" t="s">
+        <v>75</v>
+      </c>
       <c r="G93" s="4" t="s">
         <v>5</v>
       </c>
@@ -3040,30 +3059,30 @@
         <v>179</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B96" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C96" s="12" t="s">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B96" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C96" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D96" s="12" t="s">
+      <c r="D96" s="11" t="s">
         <v>129</v>
       </c>
       <c r="E96" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="F96" s="12" t="s">
+      <c r="F96" s="11" t="s">
         <v>124</v>
       </c>
       <c r="G96" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="H96" s="28" t="s">
+      <c r="H96" s="27" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B97" s="5" t="s">
         <v>134</v>
       </c>
@@ -3083,10 +3102,10 @@
       <c r="H97" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="I97" s="16"/>
-      <c r="J97" s="16"/>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I97" s="15"/>
+      <c r="J97" s="15"/>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
         <v>123</v>
       </c>
@@ -3110,7 +3129,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B99" s="5" t="s">
         <v>140</v>
       </c>
@@ -3130,34 +3149,34 @@
       <c r="H99" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="I99" s="19"/>
-      <c r="J99" s="19"/>
-      <c r="K99" s="19"/>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B102" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C102" s="12" t="s">
+      <c r="I99" s="18"/>
+      <c r="J99" s="18"/>
+      <c r="K99" s="18"/>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B102" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C102" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D102" s="12" t="s">
+      <c r="D102" s="11" t="s">
         <v>136</v>
       </c>
       <c r="E102" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="F102" s="12" t="s">
+      <c r="F102" s="11" t="s">
         <v>131</v>
       </c>
       <c r="G102" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H102" s="28" t="s">
+      <c r="H102" s="27" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B103" s="5" t="s">
         <v>141</v>
       </c>
@@ -3177,10 +3196,10 @@
       <c r="H103" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="I103" s="16"/>
-      <c r="J103" s="16"/>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I103" s="15"/>
+      <c r="J103" s="15"/>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>130</v>
       </c>
@@ -3204,7 +3223,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B105" s="5" t="s">
         <v>147</v>
       </c>
@@ -3224,34 +3243,34 @@
       <c r="H105" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="I105" s="19"/>
-      <c r="J105" s="19"/>
-      <c r="K105" s="19"/>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B108" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C108" s="12" t="s">
+      <c r="I105" s="18"/>
+      <c r="J105" s="18"/>
+      <c r="K105" s="18"/>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B108" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C108" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D108" s="12" t="s">
+      <c r="D108" s="11" t="s">
         <v>143</v>
       </c>
       <c r="E108" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="F108" s="12" t="s">
+      <c r="F108" s="11" t="s">
         <v>138</v>
       </c>
       <c r="G108" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="H108" s="28" t="s">
+      <c r="H108" s="27" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B109" s="5" t="s">
         <v>148</v>
       </c>
@@ -3271,10 +3290,10 @@
       <c r="H109" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="I109" s="16"/>
-      <c r="J109" s="16"/>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I109" s="15"/>
+      <c r="J109" s="15"/>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
         <v>137</v>
       </c>
@@ -3298,7 +3317,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B111" s="5" t="s">
         <v>152</v>
       </c>
@@ -3318,34 +3337,34 @@
       <c r="H111" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="I111" s="19"/>
-      <c r="J111" s="19"/>
-      <c r="K111" s="19"/>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B114" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C114" s="12" t="s">
+      <c r="I111" s="18"/>
+      <c r="J111" s="18"/>
+      <c r="K111" s="18"/>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B114" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C114" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D114" s="12" t="s">
+      <c r="D114" s="11" t="s">
         <v>150</v>
       </c>
       <c r="E114" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="F114" s="12" t="s">
+      <c r="F114" s="11" t="s">
         <v>145</v>
       </c>
       <c r="G114" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="H114" s="28" t="s">
+      <c r="H114" s="27" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B115" s="5" t="s">
         <v>153</v>
       </c>
@@ -3365,10 +3384,10 @@
       <c r="H115" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="I115" s="16"/>
-      <c r="J115" s="16"/>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I115" s="15"/>
+      <c r="J115" s="15"/>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
         <v>144</v>
       </c>
@@ -3392,7 +3411,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B117" s="5" t="s">
         <v>163</v>
       </c>
@@ -3412,42 +3431,42 @@
       <c r="H117" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="I117" s="19"/>
-      <c r="J117" s="19"/>
-      <c r="K117" s="19"/>
-    </row>
-    <row r="120" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C120" s="12" t="s">
+      <c r="I117" s="18"/>
+      <c r="J117" s="18"/>
+      <c r="K117" s="18"/>
+    </row>
+    <row r="120" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B120" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C120" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D120" s="21" t="s">
+      <c r="D120" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="E120" s="21" t="s">
+      <c r="E120" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="F120" s="21" t="s">
+      <c r="F120" s="20" t="s">
         <v>182</v>
       </c>
       <c r="G120" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="H120" s="12" t="s">
+      <c r="H120" s="11" t="s">
         <v>155</v>
       </c>
       <c r="I120" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="J120" s="28" t="s">
+      <c r="J120" s="27" t="s">
         <v>183</v>
       </c>
       <c r="K120" s="2"/>
       <c r="L120" s="2"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B121" s="5" t="s">
         <v>164</v>
       </c>
@@ -3460,7 +3479,7 @@
       <c r="E121" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F121" s="18">
+      <c r="F121" s="17">
         <v>42810</v>
       </c>
       <c r="G121" s="4"/>
@@ -3471,10 +3490,10 @@
       <c r="J121" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="K121" s="17"/>
-      <c r="L121" s="17"/>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K121" s="16"/>
+      <c r="L121" s="16"/>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
         <v>151</v>
       </c>
@@ -3488,10 +3507,10 @@
       <c r="D122" s="4">
         <v>1</v>
       </c>
-      <c r="E122" s="18">
+      <c r="E122" s="17">
         <v>42735</v>
       </c>
-      <c r="F122" s="18">
+      <c r="F122" s="17">
         <v>42810</v>
       </c>
       <c r="G122" s="4"/>
@@ -3505,7 +3524,7 @@
       <c r="K122" s="2"/>
       <c r="L122" s="2"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B123" s="5" t="s">
         <v>166</v>
       </c>
@@ -3525,37 +3544,37 @@
       <c r="H123" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I123" s="11"/>
+      <c r="I123" s="10"/>
       <c r="J123" s="8" t="s">
         <v>179</v>
       </c>
       <c r="K123" s="2"/>
       <c r="L123" s="2"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B126" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C126" s="12" t="s">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B126" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C126" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D126" s="12" t="s">
+      <c r="D126" s="11" t="s">
         <v>175</v>
       </c>
       <c r="E126" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="F126" s="12" t="s">
+      <c r="F126" s="11" t="s">
         <v>158</v>
       </c>
       <c r="G126" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="H126" s="28" t="s">
+      <c r="H126" s="27" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B127" s="5" t="s">
         <v>167</v>
       </c>
@@ -3576,7 +3595,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
         <v>157</v>
       </c>
@@ -3600,7 +3619,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B129" s="5" t="s">
         <v>172</v>
       </c>
@@ -3620,46 +3639,46 @@
       <c r="H129" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="I129" s="19"/>
-      <c r="J129" s="19"/>
-      <c r="K129" s="19"/>
-    </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="K131" s="31"/>
-      <c r="L131" s="31"/>
-      <c r="M131" s="31"/>
-      <c r="N131" s="31"/>
-      <c r="O131" s="27"/>
-    </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B132" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C132" s="12" t="s">
+      <c r="I129" s="18"/>
+      <c r="J129" s="18"/>
+      <c r="K129" s="18"/>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K131" s="30"/>
+      <c r="L131" s="30"/>
+      <c r="M131" s="30"/>
+      <c r="N131" s="30"/>
+      <c r="O131" s="26"/>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B132" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C132" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D132" s="12" t="s">
+      <c r="D132" s="11" t="s">
         <v>176</v>
       </c>
       <c r="E132" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="F132" s="12" t="s">
+      <c r="F132" s="11" t="s">
         <v>161</v>
       </c>
       <c r="G132" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H132" s="28" t="s">
+      <c r="H132" s="27" t="s">
         <v>183</v>
       </c>
-      <c r="K132" s="27"/>
-      <c r="L132" s="27"/>
-      <c r="M132" s="32"/>
-      <c r="N132" s="27"/>
-      <c r="O132" s="27"/>
-    </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K132" s="26"/>
+      <c r="L132" s="26"/>
+      <c r="M132" s="31"/>
+      <c r="N132" s="26"/>
+      <c r="O132" s="26"/>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B133" s="5" t="s">
         <v>173</v>
       </c>
@@ -3679,13 +3698,13 @@
       <c r="H133" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="K133" s="27"/>
-      <c r="L133" s="32"/>
-      <c r="M133" s="32"/>
-      <c r="N133" s="33"/>
-      <c r="O133" s="27"/>
-    </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K133" s="26"/>
+      <c r="L133" s="31"/>
+      <c r="M133" s="31"/>
+      <c r="N133" s="32"/>
+      <c r="O133" s="26"/>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
         <v>162</v>
       </c>
@@ -3708,13 +3727,13 @@
       <c r="H134" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="K134" s="27"/>
-      <c r="L134" s="27"/>
-      <c r="M134" s="32"/>
-      <c r="N134" s="27"/>
-      <c r="O134" s="27"/>
-    </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K134" s="26"/>
+      <c r="L134" s="26"/>
+      <c r="M134" s="31"/>
+      <c r="N134" s="26"/>
+      <c r="O134" s="26"/>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B135" s="5" t="s">
         <v>184</v>
       </c>
@@ -3735,30 +3754,30 @@
         <v>179</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B138" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C138" s="12" t="s">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B138" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C138" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D138" s="12" t="s">
+      <c r="D138" s="11" t="s">
         <v>177</v>
       </c>
       <c r="E138" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="F138" s="12" t="s">
+      <c r="F138" s="11" t="s">
         <v>170</v>
       </c>
       <c r="G138" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="H138" s="28" t="s">
+      <c r="H138" s="27" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B139" s="5" t="s">
         <v>185</v>
       </c>
@@ -3779,7 +3798,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
         <v>169</v>
       </c>
@@ -3803,7 +3822,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B141" s="5" t="s">
         <v>187</v>
       </c>

</xml_diff>